<commit_message>
Almost finished UI Inventory
</commit_message>
<xml_diff>
--- a/documents/Giphy Search Content Inventory.xlsx
+++ b/documents/Giphy Search Content Inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaredmartinez/Documents/Personal Projects/Giphy-Search/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC35BC44-83D7-5F44-A012-502C9982E7E9}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF0E217-6AB8-BB48-BC3D-29D054D9373A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>Page Title</t>
   </si>
@@ -113,7 +113,76 @@
     <t xml:space="preserve">           &lt;button&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">        </t>
+    <t>Main</t>
+  </si>
+  <si>
+    <t>&lt;main&gt;</t>
+  </si>
+  <si>
+    <t>Header of the page</t>
+  </si>
+  <si>
+    <t>To provide the page with a top section</t>
+  </si>
+  <si>
+    <t>Naviagtional Bar for the top of the page</t>
+  </si>
+  <si>
+    <t>To provide the page with a clear search place</t>
+  </si>
+  <si>
+    <t>Title for the Page</t>
+  </si>
+  <si>
+    <t>To show users what site they are on</t>
+  </si>
+  <si>
+    <t>Input field</t>
+  </si>
+  <si>
+    <t>Allows users to search</t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t>content of page</t>
+  </si>
+  <si>
+    <t>Allows users to see results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    section#gifs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    &lt;section id="gifs&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Show more Button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        &lt;button id="showMore"&gt;</t>
+  </si>
+  <si>
+    <t>Shows the gifs</t>
+  </si>
+  <si>
+    <t>Section for the gifs that are returned</t>
+  </si>
+  <si>
+    <t>Button for showing more gifs related to the search</t>
+  </si>
+  <si>
+    <t>Allows users to see more results if wanted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Footer </t>
+  </si>
+  <si>
+    <t>&lt;footer&gt;</t>
+  </si>
+  <si>
+    <t>Bottom of the page</t>
   </si>
 </sst>
 </file>
@@ -6547,7 +6616,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6571,25 +6640,33 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="26" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="26" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
@@ -6598,8 +6675,12 @@
       <c r="B4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
@@ -6608,8 +6689,12 @@
       <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
@@ -6618,33 +6703,65 @@
       <c r="B6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="A8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="26" x14ac:dyDescent="0.15">
+      <c r="A9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>